<commit_message>
agregado de tc4, td5a, instrumental 6a
</commit_message>
<xml_diff>
--- a/inasistencias-4b-tc/alumnos-4b-tc.xlsx
+++ b/inasistencias-4b-tc/alumnos-4b-tc.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="225">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -41,6 +41,9 @@
     <t xml:space="preserve">Dirección de correo</t>
   </si>
   <si>
+    <t xml:space="preserve">obs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ivan</t>
   </si>
   <si>
@@ -164,6 +167,9 @@
     <t xml:space="preserve">49837749@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Tarde 12:40</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ramiro Ezequiel</t>
   </si>
   <si>
@@ -171,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">49676837@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tade 12:45</t>
   </si>
   <si>
     <t xml:space="preserve">Benjamin</t>
@@ -776,7 +785,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -786,10 +795,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -810,7 +815,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -823,6 +828,28 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF232629"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -895,18 +922,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -925,22 +953,31 @@
       <c r="E1" s="2" t="n">
         <v>45785</v>
       </c>
+      <c r="F1" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,16 +985,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,16 +1005,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -982,16 +1025,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,16 +1045,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,16 +1065,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,16 +1085,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,16 +1105,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,16 +1125,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,16 +1145,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,16 +1165,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,16 +1185,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,16 +1205,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,16 +1228,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1169,16 +1251,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,21 +1271,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E18" s="0" t="n">
         <f aca="false">COUNTIF(E2:E17,"P")</f>
+        <v>14</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <f aca="false">COUNTIF(F2:F17,"P")</f>
         <v>14</v>
       </c>
     </row>
@@ -1223,10 +1315,10 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.21"/>
@@ -1240,46 +1332,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -1315,7 +1407,7 @@
         <f aca="false">ROUND(AVERAGE(C2,E2,G2,I2,N2),0)</f>
         <v>1</v>
       </c>
-      <c r="P2" s="4" t="str">
+      <c r="P2" s="3" t="str">
         <f aca="false">IF(O2&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1325,27 +1417,27 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="n">
         <v>9</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>45782</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="4" t="n">
         <v>4</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>45782</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="4" t="n">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="n">
         <v>45782</v>
       </c>
-      <c r="I3" s="5" t="n">
+      <c r="I3" s="4" t="n">
         <v>8</v>
       </c>
       <c r="J3" s="2" t="n">
@@ -1365,7 +1457,7 @@
         <f aca="false">ROUND(AVERAGE(C3,E3,G3,I3,N3),0)</f>
         <v>6</v>
       </c>
-      <c r="P3" s="4" t="str">
+      <c r="P3" s="3" t="str">
         <f aca="false">IF(O3&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1375,7 +1467,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>8</v>
@@ -1404,7 +1496,7 @@
         <f aca="false">ROUND(AVERAGE(C4,E4,G4,I4,N4),0)</f>
         <v>8</v>
       </c>
-      <c r="P4" s="4" t="str">
+      <c r="P4" s="3" t="str">
         <f aca="false">IF(O4&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -1414,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>10</v>
@@ -1442,7 +1534,7 @@
         <f aca="false">ROUND(AVERAGE(C5,E5,G5,I5,N5),0)</f>
         <v>7</v>
       </c>
-      <c r="P5" s="4" t="str">
+      <c r="P5" s="3" t="str">
         <f aca="false">IF(O5&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -1452,7 +1544,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>5</v>
@@ -1469,7 +1561,7 @@
       <c r="K6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="M6" s="5" t="n">
+      <c r="M6" s="4" t="n">
         <v>6</v>
       </c>
       <c r="N6" s="0" t="n">
@@ -1480,7 +1572,7 @@
         <f aca="false">ROUND(AVERAGE(C6,E6,G6,I6,N6),0)</f>
         <v>7</v>
       </c>
-      <c r="P6" s="4" t="str">
+      <c r="P6" s="3" t="str">
         <f aca="false">IF(O6&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -1490,7 +1582,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -1518,7 +1610,7 @@
         <f aca="false">ROUND(AVERAGE(C7,E7,G7,I7,N7),0)</f>
         <v>1</v>
       </c>
-      <c r="P7" s="4" t="str">
+      <c r="P7" s="3" t="str">
         <f aca="false">IF(O7&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1528,7 +1620,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>6</v>
@@ -1556,7 +1648,7 @@
         <f aca="false">ROUND(AVERAGE(C8,E8,G8,I8,N8),0)</f>
         <v>5</v>
       </c>
-      <c r="P8" s="4" t="str">
+      <c r="P8" s="3" t="str">
         <f aca="false">IF(O8&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1566,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>5</v>
@@ -1594,7 +1686,7 @@
         <f aca="false">ROUND(AVERAGE(C9,E9,G9,I9,N9),0)</f>
         <v>5</v>
       </c>
-      <c r="P9" s="4" t="str">
+      <c r="P9" s="3" t="str">
         <f aca="false">IF(O9&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1604,12 +1696,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E10" s="5" t="n">
+      <c r="E10" s="4" t="n">
         <v>5</v>
       </c>
       <c r="F10" s="2" t="n">
@@ -1618,7 +1710,7 @@
       <c r="G10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="J10" s="2" t="n">
@@ -1638,7 +1730,7 @@
         <f aca="false">ROUND(AVERAGE(C10,E10,G10,I10,N10),0)</f>
         <v>9</v>
       </c>
-      <c r="P10" s="4" t="str">
+      <c r="P10" s="3" t="str">
         <f aca="false">IF(O10&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -1648,7 +1740,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>8</v>
@@ -1677,7 +1769,7 @@
         <f aca="false">ROUND(AVERAGE(C11,E11,G11,I11,N11),0)</f>
         <v>5</v>
       </c>
-      <c r="P11" s="4" t="str">
+      <c r="P11" s="3" t="str">
         <f aca="false">IF(O11&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1687,7 +1779,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -1715,7 +1807,7 @@
         <f aca="false">ROUND(AVERAGE(C12,E12,G12,I12,N12),0)</f>
         <v>1</v>
       </c>
-      <c r="P12" s="4" t="str">
+      <c r="P12" s="3" t="str">
         <f aca="false">IF(O12&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1725,7 +1817,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>3</v>
@@ -1753,7 +1845,7 @@
         <f aca="false">ROUND(AVERAGE(C13,E13,G13,I13,N13),0)</f>
         <v>5</v>
       </c>
-      <c r="P13" s="4" t="str">
+      <c r="P13" s="3" t="str">
         <f aca="false">IF(O13&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1763,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -1791,7 +1883,7 @@
         <f aca="false">ROUND(AVERAGE(C14,E14,G14,I14,N14),0)</f>
         <v>1</v>
       </c>
-      <c r="P14" s="4" t="str">
+      <c r="P14" s="3" t="str">
         <f aca="false">IF(O14&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1801,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>8</v>
@@ -1829,7 +1921,7 @@
         <f aca="false">ROUND(AVERAGE(C15,E15,G15,I15,N15),0)</f>
         <v>2</v>
       </c>
-      <c r="P15" s="4" t="str">
+      <c r="P15" s="3" t="str">
         <f aca="false">IF(O15&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1839,7 +1931,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1</v>
@@ -1867,7 +1959,7 @@
         <f aca="false">ROUND(AVERAGE(C16,E16,G16,I16,N16),0)</f>
         <v>1</v>
       </c>
-      <c r="P16" s="4" t="str">
+      <c r="P16" s="3" t="str">
         <f aca="false">IF(O16&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -1877,7 +1969,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>9</v>
@@ -1905,7 +1997,7 @@
         <f aca="false">ROUND(AVERAGE(C17,E17,G17,I17,N17),0)</f>
         <v>8</v>
       </c>
-      <c r="P17" s="4" t="str">
+      <c r="P17" s="3" t="str">
         <f aca="false">IF(O17&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -1942,7 +2034,7 @@
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.22"/>
@@ -1953,22 +2045,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -1990,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -2004,16 +2096,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8</v>
@@ -2027,16 +2119,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>10</v>
@@ -2050,16 +2142,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>6</v>
@@ -2078,13 +2170,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>6</v>
@@ -2092,13 +2184,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>4</v>
@@ -2109,7 +2201,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -2123,16 +2215,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
@@ -2151,13 +2243,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>5</v>
@@ -2168,16 +2260,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>7</v>
@@ -2196,13 +2288,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>7</v>
@@ -2210,13 +2302,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>4</v>
@@ -2224,13 +2316,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>4</v>
@@ -2238,13 +2330,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>2</v>
@@ -2255,16 +2347,16 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>10</v>
@@ -2278,16 +2370,16 @@
         <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>8</v>
@@ -2301,7 +2393,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1</v>
@@ -2315,16 +2407,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>3</v>
@@ -2338,16 +2430,16 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -2361,16 +2453,16 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>8</v>
@@ -2384,7 +2476,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1</v>
@@ -2398,16 +2490,16 @@
         <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>9</v>
@@ -2426,13 +2518,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>8</v>
@@ -2460,7 +2552,7 @@
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.21"/>
@@ -2474,22 +2566,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,7 +2589,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -2511,7 +2603,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -2525,16 +2617,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8.7</v>
@@ -2548,16 +2640,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>5.8</v>
@@ -2576,13 +2668,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2.9</v>
@@ -2593,16 +2685,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>6.9</v>
@@ -2616,7 +2708,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
@@ -2630,16 +2722,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5.9</v>
@@ -2658,13 +2750,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>2</v>
@@ -2672,13 +2764,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0.9</v>
@@ -2689,16 +2781,16 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2.8</v>
@@ -2717,13 +2809,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0.9</v>
@@ -2734,16 +2826,16 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0.9</v>
@@ -2757,16 +2849,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>7.8</v>
@@ -2785,13 +2877,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>5.7</v>
@@ -2802,7 +2894,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
@@ -2816,7 +2908,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -2830,16 +2922,16 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>0</v>
@@ -2853,16 +2945,16 @@
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>1</v>
@@ -2876,7 +2968,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -2890,16 +2982,16 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>10</v>
@@ -2918,13 +3010,13 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>9</v>
@@ -2932,13 +3024,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>6.9</v>
@@ -2946,13 +3038,13 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>4.9</v>
@@ -2960,13 +3052,13 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>3</v>
@@ -2974,13 +3066,13 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0.9</v>
@@ -3009,7 +3101,7 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.21"/>
@@ -3022,22 +3114,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -3059,7 +3151,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -3073,16 +3165,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
@@ -3101,13 +3193,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>8</v>
@@ -3118,16 +3210,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>9</v>
@@ -3141,16 +3233,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>10</v>
@@ -3169,13 +3261,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>4</v>
@@ -3186,7 +3278,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -3200,16 +3292,16 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>8</v>
@@ -3223,16 +3315,16 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>10</v>
@@ -3251,13 +3343,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>9</v>
@@ -3268,16 +3360,16 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>10</v>
@@ -3291,16 +3383,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>10</v>
@@ -3319,13 +3411,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>3</v>
@@ -3333,13 +3425,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>3</v>
@@ -3347,13 +3439,13 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>2</v>
@@ -3361,13 +3453,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>2</v>
@@ -3378,7 +3470,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1</v>
@@ -3392,16 +3484,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>8</v>
@@ -3415,16 +3507,16 @@
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -3438,7 +3530,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1</v>
@@ -3452,7 +3544,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1</v>
@@ -3466,16 +3558,16 @@
         <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>7</v>
@@ -3509,7 +3601,7 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.21"/>
@@ -3523,22 +3615,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,7 +3638,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -3560,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -3574,16 +3666,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
@@ -3602,13 +3694,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>7</v>
@@ -3619,16 +3711,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
@@ -3642,16 +3734,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>9</v>
@@ -3665,7 +3757,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
@@ -3679,16 +3771,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>3</v>
@@ -3702,16 +3794,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>9</v>
@@ -3725,16 +3817,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>0</v>
@@ -3748,16 +3840,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>8</v>
@@ -3776,13 +3868,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>3</v>
@@ -3790,13 +3882,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>3</v>
@@ -3804,13 +3896,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2</v>
@@ -3821,7 +3913,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1</v>
@@ -3835,16 +3927,16 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>7</v>
@@ -3858,16 +3950,16 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -3881,7 +3973,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>1</v>
@@ -3895,7 +3987,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>1</v>
@@ -3909,16 +4001,16 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>6</v>
@@ -3952,7 +4044,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.21"/>
@@ -3965,22 +4057,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3988,7 +4080,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -4002,7 +4094,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
@@ -4016,16 +4108,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>1</v>
@@ -4039,16 +4131,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>6</v>
@@ -4062,16 +4154,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>4</v>
@@ -4085,16 +4177,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>2</v>
@@ -4108,16 +4200,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>4</v>
@@ -4131,7 +4223,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -4145,16 +4237,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>213</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>210</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>8</v>
@@ -4168,16 +4260,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>4</v>
@@ -4196,13 +4288,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>2</v>
@@ -4213,7 +4305,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>1</v>
@@ -4227,16 +4319,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>6</v>
@@ -4250,7 +4342,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>1</v>
@@ -4264,7 +4356,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1</v>
@@ -4278,7 +4370,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
@@ -4292,16 +4384,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>6</v>
@@ -4341,10 +4433,10 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.21"/>
@@ -4364,183 +4456,183 @@
         <v>45750</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>8</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">C2+D2</f>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">C3+D3</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">C4+D4</f>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="E5" s="0" t="n">
         <f aca="false">C5+D5</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">C6+D6</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">C7+D7</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">C8+D8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">C9+D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">C10+D10</f>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">C11+D11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="E12" s="0" t="n">
         <f aca="false">C12+D12</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -4552,10 +4644,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -4567,10 +4659,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -4582,32 +4674,32 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">C16+D16</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">C17+D17</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>